<commit_message>
The main.go file was modified.
</commit_message>
<xml_diff>
--- a/doc/Backlog.xlsx
+++ b/doc/Backlog.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gian_\OneDrive\Documentos\Proyectos\Golang\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gian_\OneDrive\Documentos\Proyectos\Golang\car-dealer-api\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Description</t>
   </si>
@@ -32,16 +32,10 @@
     <t>ID</t>
   </si>
   <si>
-    <t>1/car-model-service-repository</t>
-  </si>
-  <si>
     <t>Ticket</t>
   </si>
   <si>
     <t>About</t>
-  </si>
-  <si>
-    <t>Model, Service and Repository Entity</t>
   </si>
   <si>
     <r>
@@ -178,9 +172,6 @@
     </r>
   </si>
   <si>
-    <t>2/client-model-service-repository</t>
-  </si>
-  <si>
     <t>Configuration</t>
   </si>
   <si>
@@ -188,6 +179,80 @@
   </si>
   <si>
     <t>0/initial-setup</t>
+  </si>
+  <si>
+    <t>Car Endpoints</t>
+  </si>
+  <si>
+    <t>1/car-model-controller-routes</t>
+  </si>
+  <si>
+    <t>Documentation</t>
+  </si>
+  <si>
+    <t>3/final-documentation</t>
+  </si>
+  <si>
+    <t>Model, Controller and Routes Entity</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Car endpoints:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+POST
+GET
+GET ALL
+GET BY NAME
+PUT
+DELETE
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Documentation:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+README
+Backlog
+Technical Info</t>
+    </r>
+  </si>
+  <si>
+    <t>2/car-endpoints</t>
   </si>
 </sst>
 </file>
@@ -247,7 +312,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -255,31 +320,149 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -562,130 +745,90 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.5703125" style="7" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" style="7" customWidth="1"/>
-    <col min="3" max="3" width="31.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.5703125" style="5" customWidth="1"/>
-    <col min="5" max="16384" width="11.42578125" style="5"/>
+    <col min="1" max="1" width="7.5703125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="31.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.5703125" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="4" t="s">
+      <c r="B1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="C1" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="15" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+      <c r="A2" s="3">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>9</v>
+      <c r="B2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="123.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+      <c r="A3" s="3">
         <v>1</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="B3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
         <v>2</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>6</v>
+      <c r="B4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="2"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+    <row r="5" spans="1:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="9">
         <v>3</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>4</v>
-      </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>5</v>
-      </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>6</v>
-      </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>7</v>
-      </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>8</v>
-      </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>9</v>
-      </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
+      <c r="B5" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>14</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
The documentation was added.
</commit_message>
<xml_diff>
--- a/doc/Backlog.xlsx
+++ b/doc/Backlog.xlsx
@@ -196,11 +196,40 @@
     <t>Model, Controller and Routes Entity</t>
   </si>
   <si>
+    <t>2/car-endpoints</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
-        <sz val="11"/>
-        <color theme="1"/>
+        <sz val="14"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Documentation:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+README
+Backlog
+Technical Info</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF00B050"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -221,38 +250,8 @@
 GET ALL
 GET BY NAME
 PUT
-DELETE
-</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Documentation:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-README
-Backlog
-Technical Info</t>
-    </r>
-  </si>
-  <si>
-    <t>2/car-endpoints</t>
+DELETE</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -748,7 +747,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -774,7 +773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>0</v>
       </c>
@@ -788,7 +787,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="123.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -802,7 +801,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="126.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -810,13 +809,13 @@
         <v>8</v>
       </c>
       <c r="C4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="8" t="s">
-        <v>13</v>
-      </c>
     </row>
-    <row r="5" spans="1:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="84" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="9">
         <v>3</v>
       </c>

</xml_diff>